<commit_message>
Updated Caltech datasheet Better E2fit function
</commit_message>
<xml_diff>
--- a/public/Caltech.xlsx
+++ b/public/Caltech.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="30" sheetId="1" state="visible" r:id="rId2"/>
@@ -69,6 +69,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,6 +90,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,11 +140,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,8 +167,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -225,7 +227,7 @@
         <v>-1.997</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1.958</v>
+        <v>1.998</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.0191</v>
@@ -248,7 +250,7 @@
         <v>-1.995</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.957</v>
+        <v>1.997</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.0689</v>
@@ -271,7 +273,7 @@
         <v>-1.992</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1.956</v>
+        <v>1.996</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0.1288</v>
@@ -294,7 +296,7 @@
         <v>-1.988</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1.954</v>
+        <v>1.994</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0.1955</v>
@@ -317,7 +319,7 @@
         <v>-1.98</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1.951</v>
+        <v>1.991</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0.2754</v>
@@ -672,8 +674,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,7 +809,7 @@
         <v>-0.0553</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>1.355</v>
+        <v>1.395</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0.114</v>
@@ -824,7 +826,7 @@
         <v>-1.883</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1.227</v>
+        <v>1.837</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>-0.043</v>
@@ -847,7 +849,7 @@
         <v>-1.859</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1.216</v>
+        <v>1.816</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>-0.0289</v>
@@ -933,7 +935,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>-1.71</v>
@@ -1179,8 +1181,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1690,8 +1692,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1773,7 +1775,7 @@
         <v>-1.874</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.726</v>
+        <v>1.738</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-0.0602</v>
@@ -1842,7 +1844,7 @@
         <v>-1.825</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1.66</v>
+        <v>1.68</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>-0.0529</v>
@@ -1911,7 +1913,7 @@
         <v>-1.732</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>1.55</v>
+        <v>1.59</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>-0.0271</v>
@@ -2026,7 +2028,7 @@
         <v>-1.23</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1.254</v>
+        <v>1.292</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0.0859</v>
@@ -2043,7 +2045,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>450</v>
+        <v>490</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>-1.042</v>
@@ -2197,7 +2199,7 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2704,8 +2706,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2741,7 +2743,7 @@
         <v>-1.813</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1.468</v>
+        <v>1.488</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>-0.0415</v>
@@ -2764,7 +2766,7 @@
         <v>-1.806</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1.475</v>
+        <v>1.479</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>-0.0472</v>
@@ -2787,7 +2789,7 @@
         <v>-1.799</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.465</v>
+        <v>1.469</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-0.0505</v>
@@ -2833,7 +2835,7 @@
         <v>-1.771</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1.428</v>
+        <v>1.438</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>-0.0542</v>
@@ -3017,7 +3019,7 @@
         <v>-1.333</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>1.152</v>
+        <v>1.192</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>-0.0002</v>
@@ -3211,7 +3213,7 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -3718,8 +3720,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3755,7 +3757,7 @@
         <v>-1.996</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1.557</v>
+        <v>1.997</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>-0.0504</v>
@@ -3778,7 +3780,7 @@
         <v>-1.995</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1.556</v>
+        <v>1.996</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>-0.0155</v>
@@ -3801,7 +3803,7 @@
         <v>-1.993</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.556</v>
+        <v>1.996</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.0159</v>
@@ -3824,7 +3826,7 @@
         <v>-1.991</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1.554</v>
+        <v>1.994</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0.0651</v>
@@ -3847,7 +3849,7 @@
         <v>-1.986</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1.552</v>
+        <v>1.992</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0.1223</v>
@@ -3870,7 +3872,7 @@
         <v>-1.977</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1.568</v>
+        <v>1.988</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0.1936</v>
@@ -3893,7 +3895,7 @@
         <v>-1.966</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1.563</v>
+        <v>1.983</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0.2565</v>
@@ -3916,7 +3918,7 @@
         <v>-1.948</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1.576</v>
+        <v>1.976</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.3227</v>
@@ -3936,10 +3938,10 @@
         <v>96</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>-1.532</v>
+        <v>-1.932</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>1.565</v>
+        <v>1.969</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0.3646</v>
@@ -3962,7 +3964,7 @@
         <v>-1.908</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1.56</v>
+        <v>1.96</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0.4108</v>
@@ -3985,7 +3987,7 @@
         <v>-1.872</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>1.546</v>
+        <v>1.946</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0.4621</v>
@@ -4008,7 +4010,7 @@
         <v>-1.82</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>1.526</v>
+        <v>1.926</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0.5136</v>
@@ -4054,7 +4056,7 @@
         <v>-1.48</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1.755</v>
+        <v>1.795</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0.6667</v>
@@ -4225,7 +4227,7 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4732,8 +4734,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4769,7 +4771,7 @@
         <v>-1.991</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1.552</v>
+        <v>1.992</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>-0.0703</v>
@@ -4792,7 +4794,7 @@
         <v>-1.989</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1.551</v>
+        <v>1.991</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>-0.0528</v>
@@ -4815,7 +4817,7 @@
         <v>-1.987</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.565</v>
+        <v>1.989</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-0.0336</v>
@@ -4838,7 +4840,7 @@
         <v>-1.983</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1.587</v>
+        <v>1.987</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>-0.0032</v>
@@ -4861,7 +4863,7 @@
         <v>-1.977</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1.583</v>
+        <v>1.983</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0.0349</v>
@@ -4884,7 +4886,7 @@
         <v>-1.966</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1.578</v>
+        <v>1.978</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0.0862</v>
@@ -4907,7 +4909,7 @@
         <v>-1.952</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1.571</v>
+        <v>1.971</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0.1345</v>
@@ -4930,7 +4932,7 @@
         <v>-1.931</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1.56</v>
+        <v>1.96</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.1886</v>
@@ -4953,7 +4955,7 @@
         <v>-1.913</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>1.552</v>
+        <v>1.952</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0.2245</v>
@@ -4976,7 +4978,7 @@
         <v>-1.886</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1.929</v>
+        <v>1.939</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0.2658</v>
@@ -4999,7 +5001,7 @@
         <v>-1.846</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>1.521</v>
+        <v>1.921</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0.3134</v>
@@ -5022,7 +5024,7 @@
         <v>-1.79</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>1.856</v>
+        <v>1.896</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0.3634</v>
@@ -5137,7 +5139,7 @@
         <v>-0.545</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>1.354</v>
+        <v>1.394</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0.7078</v>
@@ -5160,7 +5162,7 @@
         <v>-0.199</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>1.282</v>
+        <v>1.283</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0.7585</v>
@@ -5239,7 +5241,7 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -5746,8 +5748,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5783,7 +5785,7 @@
         <v>-1.982</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1.581</v>
+        <v>1.981</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>-0.0748</v>
@@ -5806,7 +5808,7 @@
         <v>-1.979</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1.578</v>
+        <v>1.978</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>-0.0674</v>
@@ -5826,10 +5828,10 @@
         <v>50</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>-1.576</v>
+        <v>-1.976</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.576</v>
+        <v>1.976</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-0.0567</v>
@@ -5849,10 +5851,10 @@
         <v>56</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>-1.57</v>
+        <v>-1.97</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1.572</v>
+        <v>1.972</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>-0.0389</v>
@@ -5872,10 +5874,10 @@
         <v>64</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>-1.562</v>
+        <v>-1.962</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1.566</v>
+        <v>1.966</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>-0.0148</v>
@@ -5898,7 +5900,7 @@
         <v>-1.949</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1.558</v>
+        <v>1.958</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0.0198</v>
@@ -5918,10 +5920,10 @@
         <v>89</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>-1.922</v>
+        <v>-1.932</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1.547</v>
+        <v>1.947</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0.0543</v>
@@ -5944,7 +5946,7 @@
         <v>-1.907</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1.523</v>
+        <v>1.933</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.095</v>
@@ -5967,7 +5969,7 @@
         <v>-1.886</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>1.521</v>
+        <v>1.921</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0.1232</v>
@@ -5990,7 +5992,7 @@
         <v>-1.856</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1.504</v>
+        <v>1.904</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0.1565</v>
@@ -6200,7 +6202,7 @@
         <v>1.175</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0.6526</v>
+        <v>0.6926</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>1.116</v>
@@ -6253,8 +6255,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6760,8 +6762,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6794,10 +6796,10 @@
         <v>58.2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>-1.564</v>
+        <v>-1.964</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1.554</v>
+        <v>1.954</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>-0.0717</v>
@@ -6843,7 +6845,7 @@
         <v>-1.956</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.546</v>
+        <v>1.946</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-0.066</v>
@@ -6889,7 +6891,7 @@
         <v>-1.939</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1.531</v>
+        <v>1.931</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>-0.0427</v>
@@ -6912,7 +6914,7 @@
         <v>-1.922</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1.518</v>
+        <v>1.918</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>-0.0208</v>
@@ -6981,7 +6983,7 @@
         <v>-1.849</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>1.845</v>
+        <v>1.865</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0.0514</v>
@@ -7197,7 +7199,7 @@
         <v>1.171</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>0.655</v>
+        <v>0.695</v>
       </c>
       <c r="G19" s="1" t="n">
         <v>0.6841</v>
@@ -7267,7 +7269,7 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>